<commit_message>
second version with contact responsive and light background img
</commit_message>
<xml_diff>
--- a/audit-seo/Modèle-audit-SEO.xlsx
+++ b/audit-seo/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OpenClassrooms\Projets\P4\audit-seo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A7C017-E0B2-42EA-BBC5-3A172A8816D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0DFE16-E611-4296-A577-DB15BF91059A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="383" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="383" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEO" sheetId="1" r:id="rId1"/>
@@ -301,7 +301,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,6 +312,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF7030A0"/>
         <bgColor rgb="FF7030A0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA9E9A9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -335,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -352,6 +358,12 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -359,6 +371,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFA9E9A9"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -570,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -625,19 +642,19 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="55.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
       <c r="F2" s="5" t="s">
@@ -645,19 +662,19 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="55.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F3" s="5" t="s">
@@ -665,19 +682,19 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="55.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="7" t="s">
         <v>18</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -685,19 +702,19 @@
       </c>
     </row>
     <row r="5" spans="1:26" ht="55.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="7" t="s">
         <v>22</v>
       </c>
       <c r="F5" s="5" t="s">
@@ -765,19 +782,19 @@
       </c>
     </row>
     <row r="9" spans="1:26" ht="55.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="7" t="s">
         <v>38</v>
       </c>
       <c r="F9" s="5" t="s">
@@ -785,19 +802,19 @@
       </c>
     </row>
     <row r="10" spans="1:26" ht="55.15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="E10" s="7" t="s">
         <v>42</v>
       </c>
       <c r="F10" s="5" t="s">
@@ -1815,7 +1832,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
correction css validator with no errors
</commit_message>
<xml_diff>
--- a/audit-seo/Modèle-audit-SEO.xlsx
+++ b/audit-seo/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\OpenClassrooms\Projets\P4\audit-seo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1D2C7CF-978E-4B09-8565-22FAC678995B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42FABD2E-8BC8-40C0-976A-70F87F579FE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="383" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="383" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SEO" sheetId="1" r:id="rId1"/>
@@ -247,9 +247,6 @@
     <t>Modification du nom de ces attributs</t>
   </si>
   <si>
-    <t>Multiples labels pour des champs</t>
-  </si>
-  <si>
     <t>Il n'y a pas de labels pour les noms</t>
   </si>
   <si>
@@ -257,6 +254,9 @@
   </si>
   <si>
     <t>Ajout de labels</t>
+  </si>
+  <si>
+    <t>Labels non conformes</t>
   </si>
 </sst>
 </file>
@@ -587,8 +587,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.33203125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1832,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="A6:E6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1948,16 +1948,16 @@
         <v>52</v>
       </c>
       <c r="B6" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C6" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="D6" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="E6" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="E6" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>56</v>

</xml_diff>